<commit_message>
bắt đầu vào back
</commit_message>
<xml_diff>
--- a/ChucNang.xlsx
+++ b/ChucNang.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ngôn ngữ anh việt</t>
   </si>
@@ -49,13 +49,31 @@
   </si>
   <si>
     <t>3/9/2020 đang làm dỡ ở lại trang fontend index</t>
+  </si>
+  <si>
+    <t>ghi chú</t>
+  </si>
+  <si>
+    <t>post hiển thị bắt buộc phải có technology không sẽ bị lỗi</t>
+  </si>
+  <si>
+    <t>Chức năng</t>
+  </si>
+  <si>
+    <t>điểm danh tiếng của bài viết tính theo lượt vow của bài post + trả lời + đề xuất+ lượt xem</t>
+  </si>
+  <si>
+    <t>huy hiệu tính theo bài viết + câu trả lời : bài viết được 1 vow trở lên 1 đồng, 4 vow 1 bạc, 10 vow vàng, 20 vow bạc kim, 30 vow ruby</t>
+  </si>
+  <si>
+    <t>chức năng các nhân vật đánh giá nhau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +81,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,68 +405,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>